<commit_message>
CICD: Removed composite key in emp table -python code
</commit_message>
<xml_diff>
--- a/documentation/dataset_info.xlsx
+++ b/documentation/dataset_info.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="100" documentId="8_{712F2067-C958-4DAF-9B94-D27B9180176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A90BE3A-DF9D-4EFF-9F98-F981287A6BC1}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-315" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FD731EE6-82DA-4BBB-8826-D61F0ABDC3E8}"/>
+    <workbookView xWindow="2790" yWindow="2055" windowWidth="21600" windowHeight="11145" xr2:uid="{FD731EE6-82DA-4BBB-8826-D61F0ABDC3E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset_Info" sheetId="2" r:id="rId1"/>
@@ -713,7 +713,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -757,6 +757,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -765,36 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -829,6 +826,10 @@
 </file>
 
 <file path=xl/persons/person1.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1131,7 +1132,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4471FE68-4928-4C93-A5D9-3C8690FCA49A}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B15"/>
     </sheetView>
   </sheetViews>
@@ -1146,28 +1147,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="18"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="6" t="s">
         <v>101</v>
       </c>
@@ -1177,7 +1178,7 @@
       <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1186,36 +1187,36 @@
       <c r="C3" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="18" t="s">
         <v>109</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="27"/>
+      <c r="A4" s="25"/>
       <c r="B4" s="9" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="28" t="s">
+      <c r="D4" s="17" t="s">
         <v>83</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="20"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="27"/>
+      <c r="A5" s="25"/>
       <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
@@ -1224,28 +1225,28 @@
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
-      <c r="F5" s="20"/>
+      <c r="F5" s="18"/>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="27"/>
+      <c r="A6" s="25"/>
       <c r="B6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="17" t="s">
         <v>69</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="20"/>
+      <c r="F6" s="18"/>
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="27"/>
+      <c r="A7" s="25"/>
       <c r="B7" s="8" t="s">
         <v>25</v>
       </c>
@@ -1256,11 +1257,11 @@
       <c r="E7" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="20"/>
+      <c r="F7" s="18"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="27"/>
+      <c r="A8" s="25"/>
       <c r="B8" s="8" t="s">
         <v>26</v>
       </c>
@@ -1271,11 +1272,11 @@
       <c r="E8" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="20"/>
+      <c r="F8" s="18"/>
       <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="27"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="8" t="s">
         <v>27</v>
       </c>
@@ -1288,11 +1289,11 @@
       <c r="E9" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="20"/>
+      <c r="F9" s="18"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="27"/>
+      <c r="A10" s="25"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -1305,11 +1306,11 @@
       <c r="E10" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="20"/>
+      <c r="F10" s="18"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
+      <c r="A11" s="25"/>
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
@@ -1322,11 +1323,11 @@
       <c r="E11" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="20"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="8" t="s">
         <v>28</v>
       </c>
@@ -1339,11 +1340,11 @@
       <c r="E12" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="20"/>
+      <c r="F12" s="18"/>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="8" t="s">
         <v>29</v>
       </c>
@@ -1356,11 +1357,11 @@
       <c r="E13" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="20"/>
+      <c r="F13" s="18"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="27"/>
+      <c r="A14" s="25"/>
       <c r="B14" s="8" t="s">
         <v>30</v>
       </c>
@@ -1373,11 +1374,11 @@
       <c r="E14" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="20"/>
+      <c r="F14" s="18"/>
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="27"/>
+      <c r="A15" s="25"/>
       <c r="B15" s="8" t="s">
         <v>32</v>
       </c>
@@ -1390,11 +1391,11 @@
       <c r="E15" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="20"/>
+      <c r="F15" s="18"/>
       <c r="G15" s="3"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="25" t="s">
         <v>10</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -1409,13 +1410,13 @@
       <c r="E16" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="F16" s="18" t="s">
         <v>110</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="27"/>
+      <c r="A17" s="25"/>
       <c r="B17" s="9" t="s">
         <v>14</v>
       </c>
@@ -1428,45 +1429,45 @@
       <c r="E17" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="20"/>
+      <c r="F17" s="18"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="27"/>
+      <c r="A18" s="25"/>
       <c r="B18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="17" t="s">
         <v>158</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="20"/>
+      <c r="F18" s="18"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="9" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="28" t="s">
+      <c r="D19" s="17" t="s">
         <v>71</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="20"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="8" t="s">
         <v>17</v>
       </c>
@@ -1475,7 +1476,7 @@
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
-      <c r="F20" s="20"/>
+      <c r="F20" s="18"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1488,19 +1489,19 @@
       <c r="C21" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="17" t="s">
         <v>20</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="24" t="s">
         <v>100</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+      <c r="A22" s="23" t="s">
         <v>6</v>
       </c>
       <c r="B22" s="8" t="s">
@@ -1509,17 +1510,17 @@
       <c r="C22" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="28" t="s">
+      <c r="D22" s="17" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="26"/>
+      <c r="F22" s="24"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="8" t="s">
         <v>6</v>
       </c>
@@ -1532,11 +1533,11 @@
       <c r="E23" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="26"/>
+      <c r="F23" s="24"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+      <c r="A24" s="23" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -1551,11 +1552,11 @@
       <c r="E24" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="26"/>
+      <c r="F24" s="24"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="8" t="s">
         <v>33</v>
       </c>
@@ -1568,11 +1569,11 @@
       <c r="E25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="26"/>
+      <c r="F25" s="24"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="23" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -1587,11 +1588,11 @@
       <c r="E26" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="26"/>
+      <c r="F26" s="24"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="8" t="s">
         <v>34</v>
       </c>
@@ -1602,11 +1603,11 @@
       <c r="E27" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="26"/>
+      <c r="F27" s="24"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="23" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="8" t="s">
@@ -1621,11 +1622,11 @@
       <c r="E28" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="F28" s="26"/>
+      <c r="F28" s="24"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="8" t="s">
         <v>5</v>
       </c>
@@ -1638,11 +1639,11 @@
       <c r="E29" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="26"/>
+      <c r="F29" s="24"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="9" t="s">
         <v>36</v>
       </c>
@@ -1655,11 +1656,11 @@
       <c r="E30" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="24"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="25" t="s">
+      <c r="A31" s="23" t="s">
         <v>12</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -1674,11 +1675,11 @@
       <c r="E31" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="24"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="25"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="8" t="s">
         <v>29</v>
       </c>
@@ -1691,11 +1692,11 @@
       <c r="E32" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="26"/>
+      <c r="F32" s="24"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="25" t="s">
+      <c r="A33" s="23" t="s">
         <v>13</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -1704,17 +1705,17 @@
       <c r="C33" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="28" t="s">
+      <c r="D33" s="17" t="s">
         <v>105</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="26"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="8" t="s">
         <v>38</v>
       </c>
@@ -1727,11 +1728,11 @@
       <c r="E34" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F34" s="26"/>
+      <c r="F34" s="24"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="25"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="9" t="s">
         <v>36</v>
       </c>
@@ -1744,11 +1745,11 @@
       <c r="E35" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="26"/>
+      <c r="F35" s="24"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
+      <c r="A36" s="19" t="s">
         <v>15</v>
       </c>
       <c r="B36" s="8" t="s">
@@ -1757,30 +1758,35 @@
       <c r="C36" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="23" t="s">
+      <c r="D36" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="21" t="s">
+      <c r="F36" s="19" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="8" t="s">
         <v>15</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="24"/>
-      <c r="E37" s="24"/>
-      <c r="F37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="F3:F15"/>
     <mergeCell ref="F16:F20"/>
     <mergeCell ref="A36:A37"/>
@@ -1796,11 +1802,6 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A30"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2143,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313DDDB0-9CB0-46D1-A87D-724E95AFC555}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
CICD: PYTHON EDA CLEANING Complete
</commit_message>
<xml_diff>
--- a/documentation/dataset_info.xlsx
+++ b/documentation/dataset_info.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6241af64cff69f08/Documents/wecloudproject/DataAnalysis_SQL_PowerBI_Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="8_{712F2067-C958-4DAF-9B94-D27B9180176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A90BE3A-DF9D-4EFF-9F98-F981287A6BC1}"/>
+  <xr:revisionPtr revIDLastSave="134" documentId="8_{712F2067-C958-4DAF-9B94-D27B9180176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02CDD293-61E5-41F2-B137-D091E6461017}"/>
   <bookViews>
-    <workbookView xWindow="2790" yWindow="2055" windowWidth="21600" windowHeight="11145" xr2:uid="{FD731EE6-82DA-4BBB-8826-D61F0ABDC3E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FD731EE6-82DA-4BBB-8826-D61F0ABDC3E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset_Info" sheetId="2" r:id="rId1"/>
     <sheet name="Data Transformation Steps" sheetId="1" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="BusinessQuestions" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="198">
   <si>
     <t>Table Name</t>
   </si>
@@ -543,13 +544,100 @@
   </si>
   <si>
     <t>Load raw csv to MySql</t>
+  </si>
+  <si>
+    <t>LEGEND</t>
+  </si>
+  <si>
+    <t>Normalised Datasets</t>
+  </si>
+  <si>
+    <t>Cleaning Done In Python</t>
+  </si>
+  <si>
+    <t>Raw/De-Normalized Dataset</t>
+  </si>
+  <si>
+    <t>M/F Ratio</t>
+  </si>
+  <si>
+    <t>Challenge is to improve the Diversity/Inclusivity numbers in my organization - As these factors improve my organizations brand value and in turn will help me increase my shareholder valuation</t>
+  </si>
+  <si>
+    <t>New Hires M/F Ratio</t>
+  </si>
+  <si>
+    <t>Understand the ratio in the organization as a whole</t>
+  </si>
+  <si>
+    <t>Understand if the recruitment is progressing as per the revised plans</t>
+  </si>
+  <si>
+    <t>Existing Hires M/F ratio (&gt;2 yrs seniority)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph  </t>
+  </si>
+  <si>
+    <t>Graphs</t>
+  </si>
+  <si>
+    <t>By Region and by Ethnicity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> By Region and by Ethnicity</t>
+  </si>
+  <si>
+    <t>Show it by VP also so that I can verify if the VPs are taking the right actions</t>
+  </si>
+  <si>
+    <t>Same as above for age</t>
+  </si>
+  <si>
+    <t>Employee ct and exp</t>
+  </si>
+  <si>
+    <t>New Hires Employees ct and exp</t>
+  </si>
+  <si>
+    <t>Potential Merger Plans are in the works for the company. And the President wants to have a good overview of the following</t>
+  </si>
+  <si>
+    <t>1. Employee Turnover &amp; Retention pattern</t>
+  </si>
+  <si>
+    <t>2.  Diversity/Inclusivity numbers in the organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Advise: </t>
+  </si>
+  <si>
+    <t>develop targeted retention strategies, ensuring that crucial talent is retained during the transition, which is vital for the merged entity's stability and success.</t>
+  </si>
+  <si>
+    <t>So they have a good idea about the following and are able to take informed decision during the negociations</t>
+  </si>
+  <si>
+    <t>b) Risk Mitigation and Knowledge Preservation</t>
+  </si>
+  <si>
+    <t>a) Talent Retention and Transition</t>
+  </si>
+  <si>
+    <t>c) Integration Planning and Strategy</t>
+  </si>
+  <si>
+    <t>d) Cultural Alignment and Compatibility</t>
+  </si>
+  <si>
+    <t>e) Legal and Regulatory Considerations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -602,8 +690,16 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -634,8 +730,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4B8BBE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -673,47 +787,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -729,9 +808,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -763,18 +839,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -784,15 +848,38 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -802,6 +889,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4B8BBE"/>
       <color rgb="FFF4A696"/>
       <color rgb="FFB5CC40"/>
     </mruColors>
@@ -830,6 +918,10 @@
 </file>
 
 <file path=xl/persons/person2.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1130,10 +1222,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4471FE68-4928-4C93-A5D9-3C8690FCA49A}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B15"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,649 +1236,666 @@
     <col min="4" max="4" width="48.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="65.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="45.5703125" customWidth="1"/>
+    <col min="9" max="9" width="43.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+    <row r="1" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="F1" s="27"/>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="6" t="s">
+      <c r="F1" s="24"/>
+    </row>
+    <row r="2" spans="1:9" s="5" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="10"/>
-    </row>
-    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>109</v>
       </c>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="9" t="s">
+      <c r="H3" s="28" t="s">
+        <v>169</v>
+      </c>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="18"/>
+      <c r="F4" s="17"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="8" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="11" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="18"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="17"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="8" t="s">
+      <c r="H5" s="31"/>
+      <c r="I5" s="11" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="18"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="8" t="s">
+      <c r="H6" s="32"/>
+      <c r="I6" s="11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8" t="s">
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="18"/>
+      <c r="F7" s="17"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="8" t="s">
+      <c r="H7" s="33"/>
+      <c r="I7" s="11" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="18"/>
+      <c r="F8" s="17"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="8" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="18"/>
+      <c r="F9" s="17"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="8" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="18"/>
+      <c r="F10" s="17"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="25"/>
-      <c r="B11" s="8" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="18"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="8" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E12" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="18"/>
+      <c r="F12" s="17"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="8" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="8" t="s">
+      <c r="D13" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="18"/>
+      <c r="F13" s="17"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="8" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="8" t="s">
+      <c r="D14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="17"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="8" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="8" t="s">
+      <c r="D15" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="F15" s="18"/>
+      <c r="F15" s="17"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D16" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="F16" s="18" t="s">
+      <c r="F16" s="17" t="s">
         <v>110</v>
       </c>
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25"/>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="20"/>
+      <c r="B17" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F17" s="18"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="25"/>
-      <c r="B18" s="8" t="s">
+      <c r="A18" s="20"/>
+      <c r="B18" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="E18" s="8" t="s">
+      <c r="E18" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="F18" s="18"/>
+      <c r="F18" s="17"/>
       <c r="G18" s="3"/>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="20"/>
+      <c r="B19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="17" t="s">
+      <c r="D19" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="F19" s="18"/>
+      <c r="F19" s="17"/>
       <c r="G19" s="3"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="20"/>
+      <c r="B20" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="18"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="17"/>
       <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="8" t="s">
+      <c r="E21" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F21" s="24" t="s">
+      <c r="F21" s="19" t="s">
         <v>100</v>
       </c>
       <c r="G21" s="3"/>
     </row>
     <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="8" t="s">
+      <c r="E22" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="24"/>
+      <c r="F22" s="19"/>
       <c r="G22" s="3"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="23"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="18"/>
+      <c r="B23" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E23" s="8" t="s">
+      <c r="E23" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F23" s="24"/>
+      <c r="F23" s="19"/>
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F24" s="24"/>
+      <c r="F24" s="19"/>
       <c r="G24" s="3"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="23"/>
-      <c r="B25" s="8" t="s">
+      <c r="A25" s="18"/>
+      <c r="B25" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F25" s="24"/>
+      <c r="F25" s="19"/>
       <c r="G25" s="3"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="24"/>
+      <c r="F26" s="19"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="23"/>
-      <c r="B27" s="8" t="s">
+      <c r="A27" s="18"/>
+      <c r="B27" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8" t="s">
+      <c r="D27" s="7"/>
+      <c r="E27" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="24"/>
+      <c r="F27" s="19"/>
       <c r="G27" s="3"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F28" s="24"/>
+      <c r="F28" s="19"/>
       <c r="G28" s="3"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="23"/>
-      <c r="B29" s="8" t="s">
+      <c r="A29" s="18"/>
+      <c r="B29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="D29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F29" s="24"/>
+      <c r="F29" s="19"/>
       <c r="G29" s="3"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="18"/>
+      <c r="B30" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="D30" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="24"/>
+      <c r="F30" s="19"/>
       <c r="G30" s="3"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D31" s="8" t="s">
+      <c r="D31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="24"/>
+      <c r="F31" s="19"/>
       <c r="G31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="8" t="s">
+      <c r="A32" s="18"/>
+      <c r="B32" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="24"/>
+      <c r="F32" s="19"/>
       <c r="G32" s="3"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="23" t="s">
+      <c r="A33" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B33" s="8" t="s">
+      <c r="B33" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="D33" s="17" t="s">
+      <c r="D33" s="16" t="s">
         <v>105</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="E33" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="24"/>
+      <c r="F33" s="19"/>
       <c r="G33" s="3"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="23"/>
-      <c r="B34" s="8" t="s">
+      <c r="A34" s="18"/>
+      <c r="B34" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E34" s="8" t="s">
+      <c r="E34" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F34" s="24"/>
+      <c r="F34" s="19"/>
       <c r="G34" s="3"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="23"/>
-      <c r="B35" s="9" t="s">
+      <c r="A35" s="18"/>
+      <c r="B35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F35" s="24"/>
+      <c r="F35" s="19"/>
       <c r="G35" s="3"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="F36" s="19" t="s">
+      <c r="F36" s="25" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="8" t="s">
+      <c r="A37" s="25"/>
+      <c r="B37" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="20"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
+  <mergeCells count="21">
+    <mergeCell ref="H3:I3"/>
     <mergeCell ref="F3:F15"/>
     <mergeCell ref="F16:F20"/>
     <mergeCell ref="A36:A37"/>
@@ -1802,6 +1911,11 @@
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A28:A30"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1825,14 +1939,14 @@
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="1"/>
@@ -1865,12 +1979,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="13" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1885,7 +1999,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="13" t="s">
         <v>138</v>
       </c>
     </row>
@@ -1895,7 +2009,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="13" t="s">
         <v>137</v>
       </c>
     </row>
@@ -1915,7 +2029,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="13" t="s">
         <v>136</v>
       </c>
     </row>
@@ -1930,10 +2044,10 @@
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="11"/>
+      <c r="A27" s="10"/>
     </row>
     <row r="28" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="13" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1943,20 +2057,20 @@
       </c>
     </row>
     <row r="32" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="13" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="12" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
+      <c r="A34" s="10"/>
     </row>
     <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="13" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1966,168 +2080,168 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="11" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="12" t="s">
+      <c r="A39" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="11" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="11" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="12" t="s">
+      <c r="A41" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="12" t="s">
+      <c r="B41" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B42" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="12" t="s">
+      <c r="A43" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="12" t="s">
+      <c r="B43" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="11" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="12" t="s">
+      <c r="A45" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="11" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="15" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="15" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:1" s="11" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="14" t="s">
+    <row r="49" spans="1:1" s="10" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="16" t="s">
+      <c r="A50" s="15" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="15" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="13" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="15"/>
+      <c r="A54" s="14"/>
     </row>
     <row r="55" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="15" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="15" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="13" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
+      <c r="A59" s="14"/>
     </row>
     <row r="60" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="15" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="15" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="13" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
+      <c r="A64" s="14"/>
     </row>
     <row r="65" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="15" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="16" t="s">
+      <c r="A66" s="15" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="13" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="15"/>
+      <c r="A70" s="14"/>
     </row>
     <row r="71" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="16" t="s">
+      <c r="A71" s="15" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="16" t="s">
+      <c r="A72" s="15" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="16" t="s">
+      <c r="A73" s="15" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2141,6 +2255,153 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D543ADCD-AD55-409A-9C07-FB2078D836CA}">
+  <dimension ref="B3:D32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="156.7109375" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>185</v>
+      </c>
+      <c r="D23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>186</v>
+      </c>
+      <c r="D24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="B32" s="34" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313DDDB0-9CB0-46D1-A87D-724E95AFC555}">
   <dimension ref="A1:A10"/>
   <sheetViews>

</xml_diff>

<commit_message>
CICD: Project progress presentation complete
</commit_message>
<xml_diff>
--- a/documentation/dataset_info.xlsx
+++ b/documentation/dataset_info.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6241af64cff69f08/Documents/wecloudproject/DataAnalysis_SQL_PowerBI_Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="134" documentId="8_{712F2067-C958-4DAF-9B94-D27B9180176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02CDD293-61E5-41F2-B137-D091E6461017}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{712F2067-C958-4DAF-9B94-D27B9180176E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1EA1B0D-5089-4165-B25A-A01C7F394198}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FD731EE6-82DA-4BBB-8826-D61F0ABDC3E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FD731EE6-82DA-4BBB-8826-D61F0ABDC3E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Dataset_Info" sheetId="2" r:id="rId1"/>
     <sheet name="Data Transformation Steps" sheetId="1" r:id="rId2"/>
     <sheet name="BusinessQuestions" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId4"/>
+    <sheet name="PowerBiTransformationSteps" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="214">
   <si>
     <t>Table Name</t>
   </si>
@@ -531,15 +531,9 @@
     <t xml:space="preserve">Load only Employee &amp; BU </t>
   </si>
   <si>
-    <t>Analyse the tables toidemtify raw columns and tables</t>
-  </si>
-  <si>
     <t>Delete calculated columns from these tables</t>
   </si>
   <si>
-    <t>Don't load these tables to the report</t>
-  </si>
-  <si>
     <t xml:space="preserve">Use DAX studio to convert these raw tables to csv </t>
   </si>
   <si>
@@ -631,6 +625,60 @@
   </si>
   <si>
     <t>e) Legal and Regulatory Considerations</t>
+  </si>
+  <si>
+    <t>Computed</t>
+  </si>
+  <si>
+    <t>Can be computed later</t>
+  </si>
+  <si>
+    <t>Analyse the tables to identify raw columns and tables</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>Pull data from SQL</t>
+  </si>
+  <si>
+    <t>EDA</t>
+  </si>
+  <si>
+    <t>Clean</t>
+  </si>
+  <si>
+    <t>Load Data to SQL</t>
+  </si>
+  <si>
+    <t>PowerBI - PowerQuery</t>
+  </si>
+  <si>
+    <t>Load the cleaned primary tables into PowerQuery from SQL</t>
+  </si>
+  <si>
+    <t>Unload the raw tables &amp; Close n Apply</t>
+  </si>
+  <si>
+    <t>CreateNewTables (Use Enter Data button) - AgeGroup, EmploymentType, EthnicGroup, Gender, PayType, TerminationReason</t>
+  </si>
+  <si>
+    <t>Create Data Table using DAX (Use Modelling---&gt;New Table) and create multiple columns in this table</t>
+  </si>
+  <si>
+    <t>Check the model View and connect the Foreign Keys</t>
+  </si>
+  <si>
+    <t>Create Measure Table (Enter Data -&gt; Type table name as 'Measure'--&gt;LOAD</t>
+  </si>
+  <si>
+    <t>This creates a Measure table with a column named Column1 which you will delete later after adding measures</t>
+  </si>
+  <si>
+    <t>Goto report view &amp; add pages ----&gt; Turnover, Diversity &amp; Testing</t>
+  </si>
+  <si>
+    <t>Selec the Theme Source: https://community.fabric.microsoft.com/t5/Themes-Gallery/Superstore-Sales/td-p/3231442</t>
   </si>
 </sst>
 </file>
@@ -708,25 +756,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB5CC40"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF4A696"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,6 +775,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5AB81"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC98047"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -792,7 +840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -808,9 +856,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -833,53 +878,55 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -889,6 +936,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFC98047"/>
+      <color rgb="FFDD8047"/>
+      <color rgb="FFA5AB81"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFBFC2AD"/>
       <color rgb="FF4B8BBE"/>
       <color rgb="FFF4A696"/>
       <color rgb="FFB5CC40"/>
@@ -922,6 +974,14 @@
 </file>
 
 <file path=xl/persons/person3.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person4.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -1222,10 +1282,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4471FE68-4928-4C93-A5D9-3C8690FCA49A}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1236,7 +1296,7 @@
     <col min="4" max="4" width="48.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="65.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="45.5703125" customWidth="1"/>
-    <col min="9" max="9" width="43.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1262,655 +1322,672 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="G2" s="9"/>
+      <c r="G2" s="8"/>
     </row>
     <row r="3" spans="1:9" ht="31.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="27" t="s">
         <v>109</v>
       </c>
       <c r="G3" s="3"/>
-      <c r="H3" s="28" t="s">
+      <c r="H3" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="26"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="33"/>
+      <c r="B4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="27"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="33"/>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="27"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="10" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="33"/>
+      <c r="B6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="27"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="33"/>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="27"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="I3" s="29"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" s="7" t="s">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="33"/>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" s="27"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" s="27"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="33"/>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="27"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" s="27"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="33"/>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="27"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="27"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="33"/>
+      <c r="B14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F14" s="27"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" s="27"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="33"/>
+      <c r="B16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="27"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F17" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="33"/>
+      <c r="B18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="F18" s="27"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="33"/>
+      <c r="B19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F19" s="27"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="33"/>
+      <c r="B20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="27"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="33"/>
+      <c r="B21" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F22" s="32" t="s">
+        <v>100</v>
+      </c>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="F23" s="32"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="31"/>
+      <c r="B24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F24" s="32"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7" t="s">
+      <c r="E25" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="32"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="31"/>
+      <c r="B26" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="11" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7" t="s">
+      <c r="F26" s="32"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" s="32"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
+      <c r="B28" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F28" s="32"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="31" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="F29" s="32"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="31"/>
+      <c r="B30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="E30" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F8" s="17"/>
-      <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="F9" s="17"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="F10" s="17"/>
-      <c r="G10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E11" s="21" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" s="17"/>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="F30" s="32"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="31"/>
+      <c r="B31" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="32"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E32" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="7" t="s">
+      <c r="F32" s="32"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="31"/>
+      <c r="B33" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C33" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E33" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F13" s="17"/>
-      <c r="G13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="F33" s="32"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F34" s="32"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="31"/>
+      <c r="B35" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E35" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="F14" s="17"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="F15" s="17"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>157</v>
-      </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="B19" s="8" t="s">
+      <c r="F35" s="32"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="31"/>
+      <c r="B36" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F36" s="32"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>71</v>
-      </c>
-      <c r="E19" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="18"/>
-      <c r="B23" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="19"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="18"/>
-      <c r="B25" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F25" s="19"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26" s="19"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="18"/>
-      <c r="B27" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27" s="19"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="F28" s="19"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="18"/>
-      <c r="B29" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="19"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="18"/>
-      <c r="B30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F30" s="19"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F31" s="19"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="18"/>
-      <c r="B32" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="3"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="F33" s="19"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="19"/>
-      <c r="G34" s="3"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="18"/>
-      <c r="B35" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="F35" s="19"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
+      <c r="B37" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="28"/>
+      <c r="B38" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D36" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>116</v>
-      </c>
-      <c r="F36" s="25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="25"/>
-      <c r="B37" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="7" t="s">
+      <c r="C38" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D37" s="26"/>
-      <c r="E37" s="27"/>
-      <c r="F37" s="25"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="H3:I3"/>
-    <mergeCell ref="F3:F15"/>
-    <mergeCell ref="F16:F20"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="F36:F37"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="F21:F35"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="A3:A15"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="F3:F16"/>
+    <mergeCell ref="F17:F21"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="A34:A36"/>
+    <mergeCell ref="F22:F36"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A3:A16"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A29:A31"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1939,14 +2016,14 @@
     <col min="6" max="6" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="10" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:6" s="9" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:6" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C3" s="1"/>
@@ -1979,12 +2056,12 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="12" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="12" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1999,7 +2076,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="12" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2009,7 +2086,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>137</v>
       </c>
     </row>
@@ -2029,7 +2106,7 @@
       </c>
     </row>
     <row r="23" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="12" t="s">
         <v>136</v>
       </c>
     </row>
@@ -2044,10 +2121,10 @@
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10"/>
+      <c r="A27" s="9"/>
     </row>
     <row r="28" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>135</v>
       </c>
     </row>
@@ -2057,20 +2134,20 @@
       </c>
     </row>
     <row r="32" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="12" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="11" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
+      <c r="A34" s="9"/>
     </row>
     <row r="36" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>127</v>
       </c>
     </row>
@@ -2080,168 +2157,168 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="11" t="s">
+      <c r="A38" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="11" t="s">
+      <c r="A43" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B43" s="11" t="s">
+      <c r="B43" s="10" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B44" s="11" t="s">
+      <c r="B44" s="10" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="10" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="14" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="15" t="s">
+      <c r="A47" s="14" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:1" s="10" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+    <row r="49" spans="1:1" s="9" customFormat="1" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="12" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="14" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="14" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="12" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="14"/>
+      <c r="A54" s="13"/>
     </row>
     <row r="55" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="14" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="14" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="A58" s="12" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="13"/>
     </row>
     <row r="60" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A60" s="15" t="s">
+      <c r="A60" s="14" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="14" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="12" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="13"/>
     </row>
     <row r="65" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="14" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A66" s="15" t="s">
+      <c r="A66" s="14" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A69" s="13" t="s">
+      <c r="A69" s="12" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
+      <c r="A70" s="13"/>
     </row>
     <row r="71" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A71" s="15" t="s">
+      <c r="A71" s="14" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A72" s="15" t="s">
+      <c r="A72" s="14" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="15" t="s">
+      <c r="A73" s="14" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2258,8 +2335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D543ADCD-AD55-409A-9C07-FB2078D836CA}">
   <dimension ref="B3:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2271,129 +2348,129 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="13" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" t="s">
         <v>175</v>
-      </c>
-      <c r="D18" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D23" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="32" spans="2:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B32" s="34" t="s">
-        <v>191</v>
+      <c r="B32" s="18" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2403,65 +2480,135 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{313DDDB0-9CB0-46D1-A87D-724E95AFC555}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="73.42578125" customWidth="1"/>
+    <col min="1" max="1" width="92.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>168</v>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>